<commit_message>
integration of SQ functions
</commit_message>
<xml_diff>
--- a/data/output_data.xlsx
+++ b/data/output_data.xlsx
@@ -490,16 +490,16 @@
         <v>100</v>
       </c>
       <c r="C2" t="n">
-        <v>674</v>
+        <v>665</v>
       </c>
       <c r="D2" t="n">
         <v>2000</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -508,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
just small syntax changes
</commit_message>
<xml_diff>
--- a/data/output_data.xlsx
+++ b/data/output_data.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Output Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,32 +451,127 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>R4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>R5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>R6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>R7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>R8</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>R20</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>R21</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>R22</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>R23</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>R21'</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>R22'</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>R23'</t>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>R24</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>R25</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>R26</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>R20X</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>R21X</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>R22X</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>R23X</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>R24X</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>R25X</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>R8X</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>R26X</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>R2X</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>R3X</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>R4X</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>R5X</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>R6X</t>
         </is>
       </c>
     </row>
@@ -499,18 +594,75 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
         <v>7</v>
       </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
         <v>10</v>
       </c>
-      <c r="I2" t="n">
+      <c r="S2" t="n">
         <v>5</v>
       </c>
-      <c r="J2" t="n">
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -547,6 +699,63 @@
       <c r="J3" t="n">
         <v>0</v>
       </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -567,18 +776,75 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
         <v>3</v>
       </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -615,6 +881,63 @@
       <c r="J5" t="n">
         <v>0</v>
       </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -649,8 +972,65 @@
       <c r="J6" t="n">
         <v>0</v>
       </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
undiscounted reward, discounted reward, country prob, schedule prob, and expected utility
</commit_message>
<xml_diff>
--- a/data/output_data.xlsx
+++ b/data/output_data.xlsx
@@ -585,7 +585,7 @@
         <v>100</v>
       </c>
       <c r="C2" t="n">
-        <v>665</v>
+        <v>700</v>
       </c>
       <c r="D2" t="n">
         <v>2000</v>
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -630,10 +630,10 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -794,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
trying to get positive utility still lol
</commit_message>
<xml_diff>
--- a/data/output_data.xlsx
+++ b/data/output_data.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Output Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC6"/>
+  <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,132 +446,137 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>R2X</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>R3</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>R3X</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>R4</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>R4X</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>R5</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>R5X</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>R6</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>R6X</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>R7</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>R7X</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>R8</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>R8X</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>R20</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>R20X</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>R21</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>R21X</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>R22</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>R22X</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>R23</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>R23X</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>R24</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>R24X</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>R25</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>R25X</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>R26</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>R20X</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>R21X</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>R22X</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>R23X</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>R24X</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>R25X</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>R8X</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>R26X</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>R2X</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>R3X</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>R4X</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>R5X</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>R6X</t>
         </is>
       </c>
     </row>
@@ -588,19 +593,19 @@
         <v>30</v>
       </c>
       <c r="D2" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>30</v>
       </c>
       <c r="F2" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>30</v>
       </c>
       <c r="H2" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>30</v>
@@ -609,19 +614,19 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -663,6 +668,9 @@
         <v>0</v>
       </c>
       <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -679,19 +687,19 @@
         <v>11</v>
       </c>
       <c r="D3" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>11</v>
       </c>
       <c r="F3" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>11</v>
       </c>
       <c r="H3" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>11</v>
@@ -700,19 +708,19 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
@@ -754,6 +762,9 @@
         <v>0</v>
       </c>
       <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -770,19 +781,19 @@
         <v>11</v>
       </c>
       <c r="D4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>11</v>
       </c>
       <c r="F4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>11</v>
       </c>
       <c r="H4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
         <v>11</v>
@@ -791,19 +802,19 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
@@ -845,6 +856,9 @@
         <v>0</v>
       </c>
       <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -861,19 +875,19 @@
         <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>11</v>
       </c>
       <c r="F5" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>11</v>
       </c>
       <c r="H5" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>11</v>
@@ -882,19 +896,19 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -936,6 +950,9 @@
         <v>0</v>
       </c>
       <c r="AC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -952,19 +969,19 @@
         <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>11</v>
       </c>
       <c r="F6" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>11</v>
       </c>
       <c r="H6" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>11</v>
@@ -973,19 +990,19 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
@@ -1027,10 +1044,13 @@
         <v>0</v>
       </c>
       <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on waste stuff
</commit_message>
<xml_diff>
--- a/data/output_data.xlsx
+++ b/data/output_data.xlsx
@@ -88,10 +88,10 @@
     <t>Expected Utility: 5.472116134447312</t>
   </si>
   <si>
-    <t>Expected Utility: 5.34296865663645</t>
-  </si>
-  <si>
-    <t>Expected Utility: 5.21822888677308</t>
+    <t>Expected Utility: 5.33770047422445</t>
+  </si>
+  <si>
+    <t>Expected Utility: 5.171968637050121</t>
   </si>
   <si>
     <t>(TRANSFORM self (INPUTS (Population 5) (MetallicElements 3) (MetallicAlloys 2))(OUTPUTS (Population 5) (Electronics 2) (ElectonicsWaste 1))) EU: 0.22096544749376096</t>
@@ -186,7 +186,7 @@
   </si>
   <si>
     <t xml:space="preserve">
-(TRANSFER self Foremz ((Electronics 1)) EU: -0.057523822012224654</t>
+(TRANSFER self Foremz ((Electronics 1)) EU: -0.43696381975762977</t>
   </si>
 </sst>
 </file>

</xml_diff>